<commit_message>
atualizei o design das atas
</commit_message>
<xml_diff>
--- a/Pesquisa e Inovação/ATA's de Reunião/20210823_Protocolo_Reunião_Geli's.xlsx
+++ b/Pesquisa e Inovação/ATA's de Reunião/20210823_Protocolo_Reunião_Geli's.xlsx
@@ -234,18 +234,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE7F1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF421F49"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -253,6 +241,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE90949"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,38 +458,60 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -520,12 +542,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -547,64 +563,48 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -615,16 +615,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE90949"/>
+      <color rgb="FFD91954"/>
       <color rgb="FF56A44F"/>
       <color rgb="FF258A14"/>
       <color rgb="FFFFE7F1"/>
       <color rgb="FF421F49"/>
       <color rgb="FFF6C6DC"/>
       <color rgb="FFD3C8D6"/>
-      <color rgb="FFD91954"/>
       <color rgb="FFAC61BB"/>
       <color rgb="FFA14CB2"/>
-      <color rgb="FFE3E49C"/>
     </mruColors>
   </colors>
   <extLst>
@@ -643,19 +643,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>34482</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>141652</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="4" name="Imagem 3" descr="Desenho com traços pretos em fundo branco&#10;&#10;Descrição gerada automaticamente com confiança baixa">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" id="{71756BF8-A283-4F27-B2A8-51EBC71121CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -668,8 +674,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1800225" y="415482"/>
-          <a:ext cx="2505076" cy="1108518"/>
+          <a:off x="1952625" y="390525"/>
+          <a:ext cx="2038350" cy="1084627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J17"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,131 +997,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="6"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="6"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="54"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="6"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="6"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="54"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="6"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="54"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="54"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="6"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="54"/>
     </row>
     <row r="9" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="32" t="s">
         <v>14</v>
       </c>
@@ -1124,59 +1130,59 @@
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
-      <c r="K10" s="6"/>
+      <c r="K10" s="54"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="41" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="35" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="6"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="54"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="54"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34">
+      <c r="C13" s="58"/>
+      <c r="D13" s="52">
         <v>44431</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="32" t="s">
         <v>4</v>
       </c>
@@ -1188,103 +1194,103 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="54"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="52" t="s">
+      <c r="A15" s="49"/>
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="38"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="38"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="6"/>
+      <c r="K15" s="54"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="49"/>
+      <c r="B16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="6"/>
+      <c r="K16" s="54"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="49" t="s">
+      <c r="A17" s="49"/>
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="54"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="6"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="54"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="6"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="54"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="6"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="54"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="23" t="s">
         <v>24</v>
       </c>
@@ -1294,12 +1300,12 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="6"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="54"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="26"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
@@ -1307,12 +1313,12 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="6"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="54"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="26"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -1320,12 +1326,12 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="6"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="54"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="26"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -1333,12 +1339,12 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="28"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="54"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="26"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -1346,12 +1352,12 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
       <c r="I25" s="28"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="6"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="54"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="26"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -1359,12 +1365,12 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="6"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="54"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="26"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
@@ -1372,12 +1378,12 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="6"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="54"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
@@ -1385,12 +1391,12 @@
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="6"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="54"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="29"/>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
@@ -1398,294 +1404,294 @@
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
       <c r="I29" s="31"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="6"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="54"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="6"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="54"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="58" t="s">
+      <c r="A31" s="49"/>
+      <c r="B31" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="6"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="54"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="59" t="s">
+      <c r="A32" s="49"/>
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60" t="s">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="60"/>
-      <c r="I32" s="61" t="s">
+      <c r="H32" s="14"/>
+      <c r="I32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="61"/>
-      <c r="K32" s="6"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="54"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="48" t="s">
+      <c r="A33" s="49"/>
+      <c r="B33" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="46" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="42">
+      <c r="H33" s="17"/>
+      <c r="I33" s="18">
         <v>44431</v>
       </c>
-      <c r="J33" s="42"/>
-      <c r="K33" s="6"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="54"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="6"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="54"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="6"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="54"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="48" t="s">
+      <c r="A36" s="49"/>
+      <c r="B36" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="46" t="s">
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="42">
+      <c r="H36" s="17"/>
+      <c r="I36" s="18">
         <v>44431</v>
       </c>
-      <c r="J36" s="42"/>
-      <c r="K36" s="6"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="54"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="6"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="54"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="6"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="54"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="47" t="s">
+      <c r="A39" s="49"/>
+      <c r="B39" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="44" t="s">
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="44"/>
-      <c r="I39" s="45">
+      <c r="H39" s="20"/>
+      <c r="I39" s="11">
         <v>44431</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="6"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="54"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="6"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="54"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="6"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="54"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="47" t="s">
+      <c r="A42" s="49"/>
+      <c r="B42" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="54" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="54"/>
-      <c r="I42" s="45">
+      <c r="H42" s="10"/>
+      <c r="I42" s="11">
         <v>44432</v>
       </c>
-      <c r="J42" s="45"/>
-      <c r="K42" s="6"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="54"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="6"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="54"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="6"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="54"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="6"/>
+      <c r="A45" s="49"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="54"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="6"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="54"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="6"/>
+      <c r="A47" s="49"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="54"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="56" t="s">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="34">
+      <c r="C48" s="51"/>
+      <c r="D48" s="52">
         <v>44435</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="6"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="54"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="55"/>
       <c r="C49" s="55"/>
       <c r="D49" s="55"/>
@@ -1694,24 +1700,51 @@
       <c r="G49" s="55"/>
       <c r="H49" s="55"/>
       <c r="I49" s="55"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="6"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="54"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="14"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C21:I29"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="E11:J12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="I33:J35"/>
+    <mergeCell ref="B45:F47"/>
+    <mergeCell ref="G45:H47"/>
+    <mergeCell ref="I45:J47"/>
+    <mergeCell ref="G36:H38"/>
+    <mergeCell ref="I36:J38"/>
+    <mergeCell ref="B39:F41"/>
+    <mergeCell ref="G39:H41"/>
+    <mergeCell ref="I39:J41"/>
+    <mergeCell ref="B42:F44"/>
+    <mergeCell ref="B36:F38"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G42:H44"/>
@@ -1728,33 +1761,6 @@
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="B33:F35"/>
     <mergeCell ref="G33:H35"/>
-    <mergeCell ref="I33:J35"/>
-    <mergeCell ref="B45:F47"/>
-    <mergeCell ref="G45:H47"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="G36:H38"/>
-    <mergeCell ref="I36:J38"/>
-    <mergeCell ref="B39:F41"/>
-    <mergeCell ref="G39:H41"/>
-    <mergeCell ref="I39:J41"/>
-    <mergeCell ref="B42:F44"/>
-    <mergeCell ref="B36:F38"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C21:I29"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="E11:J12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B11:D12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>